<commit_message>
report: Generate graphs using octave.
</commit_message>
<xml_diff>
--- a/experiments/brightness vs temperature/temperature vs brightness.xlsx
+++ b/experiments/brightness vs temperature/temperature vs brightness.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="10">
   <si>
     <t xml:space="preserve">Brightness (%)</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve">temperature  rise (C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\</t>
   </si>
 </sst>
 </file>
@@ -229,7 +235,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -622,11 +628,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46459798"/>
-        <c:axId val="45251340"/>
+        <c:axId val="13799383"/>
+        <c:axId val="13033937"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46459798"/>
+        <c:axId val="13799383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,12 +678,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45251340"/>
+        <c:crossAx val="13033937"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45251340"/>
+        <c:axId val="13033937"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +729,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46459798"/>
+        <c:crossAx val="13799383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -751,7 +757,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -919,11 +925,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33586997"/>
-        <c:axId val="90256000"/>
+        <c:axId val="3616357"/>
+        <c:axId val="49714649"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33586997"/>
+        <c:axId val="3616357"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,12 +975,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90256000"/>
+        <c:crossAx val="49714649"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90256000"/>
+        <c:axId val="49714649"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1026,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33586997"/>
+        <c:crossAx val="3616357"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1059,9 +1065,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>28080</xdr:colOff>
+      <xdr:colOff>27720</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1069,8 +1075,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3933720" y="6314760"/>
-        <a:ext cx="4495320" cy="2742840"/>
+        <a:off x="3876480" y="6314760"/>
+        <a:ext cx="4418640" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1094,9 +1100,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>428400</xdr:colOff>
+      <xdr:colOff>428040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1104,8 +1110,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4086000" y="790200"/>
-        <a:ext cx="4505040" cy="2743200"/>
+        <a:off x="4028760" y="790200"/>
+        <a:ext cx="4438080" cy="2742840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1126,13 +1132,13 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="A22:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,12 +1388,12 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D99" activeCellId="0" sqref="D99"/>
+      <selection pane="topLeft" activeCell="D99" activeCellId="1" sqref="A22:D30 D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,12 +2468,12 @@
   <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D111" activeCellId="0" sqref="D111"/>
+      <selection pane="topLeft" activeCell="D111" activeCellId="1" sqref="A22:D30 D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,18 +3677,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A5:C14"/>
+  <dimension ref="A5:D30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,6 +3808,150 @@
       <c r="C14" s="1" t="n">
         <f aca="false">'100%'!D110</f>
         <v>44.75</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <f aca="false">A6</f>
+        <v>0.09</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <f aca="false">C6</f>
+        <v>2.17647058823529</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <f aca="false">A7</f>
+        <v>0.49</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <f aca="false">C7</f>
+        <v>6.41666666666666</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <f aca="false">A8</f>
+        <v>1.24</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">C8</f>
+        <v>11.75</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <f aca="false">A9</f>
+        <v>1.95</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">C9</f>
+        <v>17.6666666666667</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <f aca="false">A10</f>
+        <v>3.38</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <f aca="false">C10</f>
+        <v>28.0833333333333</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <f aca="false">A11</f>
+        <v>4.1</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <f aca="false">C11</f>
+        <v>29.6666666666667</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <f aca="false">A12</f>
+        <v>5.35</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <f aca="false">C12</f>
+        <v>39</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <f aca="false">A13</f>
+        <v>6</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <f aca="false">C13</f>
+        <v>43.0909090909091</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <f aca="false">A14</f>
+        <v>6.55</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <f aca="false">C14</f>
+        <v>44.75</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3824,12 +3974,12 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="A22:D30 B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,12 +4560,12 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61"/>
+      <selection pane="topLeft" activeCell="B61" activeCellId="1" sqref="A22:D30 B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,12 +5233,12 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
+      <selection pane="topLeft" activeCell="D77" activeCellId="1" sqref="A22:D30 D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5921,12 +6071,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:D30 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5947,12 +6097,12 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D99" activeCellId="0" sqref="D99"/>
+      <selection pane="topLeft" activeCell="D99" activeCellId="1" sqref="A22:D30 D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7027,12 +7177,12 @@
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D88" activeCellId="0" sqref="D88"/>
+      <selection pane="topLeft" activeCell="D88" activeCellId="1" sqref="A22:D30 D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7975,12 +8125,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A22:D30 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8001,12 +8151,12 @@
   <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
+      <selection pane="topLeft" activeCell="D120" activeCellId="1" sqref="A22:D30 D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>